<commit_message>
Automatically attempt to fix corrupt excel manual annotation files; related to #649
</commit_message>
<xml_diff>
--- a/wbfm/notebooks/paper/supplement/ids/ids_per_dataset_type.xlsx
+++ b/wbfm/notebooks/paper/supplement/ids/ids_per_dataset_type.xlsx
@@ -446,194 +446,194 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>IL2LL</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>IL2LR</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IL1LL</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IL1LR</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>RIBL</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>AWBR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>RIBR</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>AWBR</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>VA02</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>VB03</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>VB01</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>VA01</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>SIADR</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>SIADL</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>VA02</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>VB03</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>VB01</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>SIADR</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>VA01</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>RIAL</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>DB02</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>DB01</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>DD01</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>RIMR</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>RIAR</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>RIML</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>SMDVL</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>RIML</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>AVEL</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>SAAVL</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>URXR</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>DA01</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>RMDDR</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>RIS</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>DA01</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>RMDDR</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>URXR</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>SAAVR</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>URXL</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>SAAVR</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>RMDDL</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>AQR</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>AVER</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>SMDDL</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>IL1LR</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>IL2LR</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>IL2LL</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>AVBR</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>IL1LL</t>
-        </is>
-      </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
+          <t>SMDDR</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>SMDVR</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>RIVR</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
           <t>AVBL</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>SMDDR</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>RIVR</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>SMDVR</t>
-        </is>
-      </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>RMEL</t>
@@ -661,64 +661,64 @@
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
+          <t>URYVL</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>URADL</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>SIAVR</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
           <t>URYDR</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>URADL</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>URYVL</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>ALA</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>SIAVR</t>
-        </is>
-      </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
+          <t>URYVR</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>RMDVR</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>SIAVL</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
           <t>RMEV</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>URYDL</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>SIAVL</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>URYVR</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>RMDVR</t>
-        </is>
-      </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
+          <t>RMDVL</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
           <t>RMED</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>RMDVL</t>
-        </is>
-      </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>URADR</t>
@@ -726,22 +726,22 @@
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
+          <t>VB02</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
           <t>AVAR</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>VB02</t>
-        </is>
-      </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
+          <t>RMER</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
           <t>RID</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>RMER</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
@@ -760,106 +760,106 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
         <v>12</v>
       </c>
-      <c r="E2" t="n">
+      <c r="I2" t="n">
         <v>12</v>
       </c>
-      <c r="F2" t="n">
+      <c r="J2" t="n">
         <v>15</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>15</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
         <v>15</v>
       </c>
-      <c r="I2" t="n">
-        <v>15</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>16</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>16</v>
       </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
+        <v>16</v>
+      </c>
+      <c r="P2" t="n">
         <v>17</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q2" t="n">
         <v>18</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>18</v>
       </c>
-      <c r="O2" t="n">
+      <c r="S2" t="n">
         <v>19</v>
       </c>
-      <c r="P2" t="n">
+      <c r="T2" t="n">
+        <v>19</v>
+      </c>
+      <c r="U2" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" t="n">
-        <v>20</v>
-      </c>
-      <c r="R2" t="n">
+      <c r="V2" t="n">
         <v>21</v>
       </c>
-      <c r="S2" t="n">
+      <c r="W2" t="n">
         <v>21</v>
       </c>
-      <c r="T2" t="n">
+      <c r="X2" t="n">
         <v>22</v>
       </c>
-      <c r="U2" t="n">
+      <c r="Y2" t="n">
         <v>23</v>
       </c>
-      <c r="V2" t="n">
+      <c r="Z2" t="n">
         <v>24</v>
       </c>
-      <c r="W2" t="n">
+      <c r="AA2" t="n">
         <v>24</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AB2" t="n">
         <v>24</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AC2" t="n">
         <v>24</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AD2" t="n">
         <v>25</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AE2" t="n">
         <v>25</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AF2" t="n">
         <v>25</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AG2" t="n">
         <v>26</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AH2" t="n">
         <v>26</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AI2" t="n">
         <v>27</v>
       </c>
-      <c r="AF2" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG2" t="n">
+      <c r="AJ2" t="n">
         <v>28</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>28</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>28</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>29</v>
       </c>
       <c r="AK2" t="n">
         <v>30</v>
@@ -965,19 +965,19 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -1019,10 +1019,10 @@
         <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
@@ -1037,100 +1037,100 @@
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AF3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
         <v>6</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>8</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>8</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>8</v>
+      </c>
+      <c r="BH3" t="n">
         <v>5</v>
       </c>
-      <c r="AI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>8</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>8</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>6</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG3" t="n">
+      <c r="BI3" t="n">
         <v>5</v>
       </c>
-      <c r="BH3" t="n">
-        <v>8</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>8</v>
-      </c>
       <c r="BJ3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BK3" t="n">
         <v>8</v>
@@ -1146,76 +1146,76 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
         <v>6</v>
       </c>
-      <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" t="n">
-        <v>10</v>
-      </c>
-      <c r="H4" t="n">
-        <v>7</v>
-      </c>
-      <c r="I4" t="n">
-        <v>8</v>
-      </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2</v>
+      </c>
+      <c r="P4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>7</v>
+      </c>
+      <c r="R4" t="n">
         <v>5</v>
       </c>
-      <c r="O4" t="n">
-        <v>4</v>
-      </c>
-      <c r="P4" t="n">
+      <c r="S4" t="n">
+        <v>4</v>
+      </c>
+      <c r="T4" t="n">
         <v>9</v>
       </c>
-      <c r="Q4" t="n">
-        <v>10</v>
-      </c>
-      <c r="R4" t="n">
-        <v>9</v>
-      </c>
-      <c r="S4" t="n">
-        <v>9</v>
-      </c>
-      <c r="T4" t="n">
-        <v>10</v>
-      </c>
       <c r="U4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="V4" t="n">
         <v>9</v>
       </c>
       <c r="W4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Y4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AA4" t="n">
         <v>10</v>
@@ -1230,28 +1230,28 @@
         <v>10</v>
       </c>
       <c r="AE4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AF4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ4" t="n">
         <v>9</v>
       </c>
-      <c r="AG4" t="n">
-        <v>9</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>9</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>8</v>
-      </c>
       <c r="AK4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AL4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AM4" t="n">
         <v>9</v>
@@ -1281,16 +1281,16 @@
         <v>10</v>
       </c>
       <c r="AV4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AW4" t="n">
         <v>10</v>
       </c>
       <c r="AX4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AY4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AZ4" t="n">
         <v>10</v>
@@ -1299,16 +1299,16 @@
         <v>9</v>
       </c>
       <c r="BB4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BC4" t="n">
         <v>10</v>
       </c>
       <c r="BD4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE4" t="n">
         <v>9</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>10</v>
       </c>
       <c r="BF4" t="n">
         <v>10</v>
@@ -1339,94 +1339,94 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N5" t="n">
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
         <v>3</v>
       </c>
       <c r="AF5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="n">
         <v>4</v>
@@ -1435,13 +1435,13 @@
         <v>4</v>
       </c>
       <c r="AI5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ5" t="n">
         <v>4</v>
       </c>
       <c r="AK5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL5" t="n">
         <v>4</v>
@@ -1450,7 +1450,7 @@
         <v>4</v>
       </c>
       <c r="AN5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AO5" t="n">
         <v>4</v>
@@ -1474,19 +1474,19 @@
         <v>4</v>
       </c>
       <c r="AV5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AW5" t="n">
         <v>4</v>
       </c>
       <c r="AX5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AY5" t="n">
         <v>4</v>
       </c>
       <c r="AZ5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BA5" t="n">
         <v>0</v>
@@ -1495,13 +1495,13 @@
         <v>4</v>
       </c>
       <c r="BC5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BD5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BE5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BF5" t="n">
         <v>4</v>
@@ -1513,10 +1513,10 @@
         <v>4</v>
       </c>
       <c r="BI5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BJ5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BK5" t="n">
         <v>4</v>
@@ -1535,109 +1535,109 @@
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
         <v>6</v>
       </c>
-      <c r="Q6" t="n">
-        <v>2</v>
-      </c>
-      <c r="R6" t="n">
-        <v>7</v>
-      </c>
-      <c r="S6" t="n">
-        <v>8</v>
-      </c>
-      <c r="T6" t="n">
-        <v>8</v>
-      </c>
       <c r="U6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V6" t="n">
+        <v>8</v>
+      </c>
+      <c r="W6" t="n">
+        <v>7</v>
+      </c>
+      <c r="X6" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="n">
         <v>6</v>
       </c>
-      <c r="W6" t="n">
-        <v>3</v>
-      </c>
-      <c r="X6" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>10</v>
-      </c>
       <c r="AD6" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AE6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI6" t="n">
         <v>6</v>
       </c>
-      <c r="AF6" t="n">
-        <v>9</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>9</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>8</v>
-      </c>
       <c r="AJ6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AK6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AM6" t="n">
         <v>7</v>
@@ -1667,49 +1667,49 @@
         <v>5</v>
       </c>
       <c r="AV6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AW6" t="n">
+        <v>8</v>
+      </c>
+      <c r="AX6" t="n">
         <v>9</v>
       </c>
-      <c r="AX6" t="n">
-        <v>4</v>
-      </c>
       <c r="AY6" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AZ6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BA6" t="n">
         <v>4</v>
       </c>
       <c r="BB6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="BC6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BD6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BE6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BF6" t="n">
         <v>6</v>
       </c>
       <c r="BG6" t="n">
+        <v>8</v>
+      </c>
+      <c r="BH6" t="n">
         <v>9</v>
       </c>
-      <c r="BH6" t="n">
-        <v>8</v>
-      </c>
       <c r="BI6" t="n">
+        <v>7</v>
+      </c>
+      <c r="BJ6" t="n">
         <v>9</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>7</v>
       </c>
       <c r="BK6" t="n">
         <v>10</v>
@@ -1725,58 +1725,58 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
         <v>3</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U7" t="n">
         <v>1</v>
@@ -1785,19 +1785,19 @@
         <v>3</v>
       </c>
       <c r="W7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB7" t="n">
         <v>4</v>
@@ -1806,37 +1806,37 @@
         <v>3</v>
       </c>
       <c r="AD7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE7" t="n">
         <v>4</v>
       </c>
       <c r="AF7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AJ7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AM7" t="n">
         <v>3</v>
       </c>
       <c r="AN7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO7" t="n">
         <v>0</v>
@@ -1854,40 +1854,40 @@
         <v>4</v>
       </c>
       <c r="AT7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AU7" t="n">
         <v>1</v>
       </c>
       <c r="AV7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AW7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AX7" t="n">
         <v>4</v>
       </c>
       <c r="AY7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AZ7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BA7" t="n">
         <v>4</v>
       </c>
       <c r="BB7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BC7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BD7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BE7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BF7" t="n">
         <v>3</v>
@@ -1899,10 +1899,10 @@
         <v>4</v>
       </c>
       <c r="BI7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BK7" t="n">
         <v>4</v>
@@ -1918,100 +1918,100 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
         <v>5</v>
       </c>
-      <c r="H8" t="n">
+      <c r="K8" t="n">
         <v>6</v>
       </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y8" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB8" t="n">
         <v>0</v>
       </c>
       <c r="AC8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AD8" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="n">
         <v>5</v>
       </c>
       <c r="AH8" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AI8" t="n">
         <v>5</v>
@@ -2023,13 +2023,13 @@
         <v>4</v>
       </c>
       <c r="AL8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AM8" t="n">
         <v>1</v>
       </c>
       <c r="AN8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AO8" t="n">
         <v>6</v>
@@ -2047,19 +2047,19 @@
         <v>5</v>
       </c>
       <c r="AT8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AU8" t="n">
         <v>6</v>
       </c>
       <c r="AV8" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AW8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AX8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AY8" t="n">
         <v>6</v>
@@ -2077,25 +2077,25 @@
         <v>7</v>
       </c>
       <c r="BD8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BE8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BF8" t="n">
         <v>7</v>
       </c>
       <c r="BG8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BH8" t="n">
+        <v>7</v>
+      </c>
+      <c r="BI8" t="n">
         <v>6</v>
       </c>
-      <c r="BI8" t="n">
-        <v>7</v>
-      </c>
       <c r="BJ8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BK8" t="n">
         <v>7</v>

</xml_diff>